<commit_message>
Update town_lv1size from 30x20 to 30x25. Add player transfer and other events
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="208">
   <si>
     <t>Name:</t>
   </si>
@@ -801,11 +801,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30x20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Exterior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30x25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傳送點-去Town_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1172,7 +1192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -2092,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2205,6 +2225,23 @@
         <v>197</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2216,7 +2253,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2238,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2246,7 +2283,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First night in officerhouse cut scene. Add event and switch.
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,31 +4,32 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
     <sheet name="MystForst01" sheetId="2" r:id="rId2"/>
     <sheet name="Town_lv1" sheetId="3" r:id="rId3"/>
-    <sheet name="StorageShack" sheetId="4" r:id="rId4"/>
-    <sheet name="MinatoPort" sheetId="5" r:id="rId5"/>
-    <sheet name="MinatoWeaponShop" sheetId="6" r:id="rId6"/>
-    <sheet name="MinatoInn" sheetId="7" r:id="rId7"/>
-    <sheet name="MinatoItemShop" sheetId="8" r:id="rId8"/>
-    <sheet name="WorldMap1" sheetId="9" r:id="rId9"/>
-    <sheet name="CoD_F1" sheetId="10" r:id="rId10"/>
-    <sheet name="CoD_F2" sheetId="11" r:id="rId11"/>
-    <sheet name="Dungeon1" sheetId="13" r:id="rId12"/>
-    <sheet name="LavaCave" sheetId="14" r:id="rId13"/>
-    <sheet name="GoodKingsRoom" sheetId="15" r:id="rId14"/>
-    <sheet name="Switch" sheetId="12" r:id="rId15"/>
+    <sheet name="Town_lv1-1stNight" sheetId="16" r:id="rId4"/>
+    <sheet name="OfficerHouse-1stNight" sheetId="4" r:id="rId5"/>
+    <sheet name="MinatoPort" sheetId="5" r:id="rId6"/>
+    <sheet name="MinatoWeaponShop" sheetId="6" r:id="rId7"/>
+    <sheet name="MinatoInn" sheetId="7" r:id="rId8"/>
+    <sheet name="MinatoItemShop" sheetId="8" r:id="rId9"/>
+    <sheet name="WorldMap1" sheetId="9" r:id="rId10"/>
+    <sheet name="CoD_F1" sheetId="10" r:id="rId11"/>
+    <sheet name="CoD_F2" sheetId="11" r:id="rId12"/>
+    <sheet name="Dungeon1" sheetId="13" r:id="rId13"/>
+    <sheet name="LavaCave" sheetId="14" r:id="rId14"/>
+    <sheet name="GoodKingsRoom" sheetId="15" r:id="rId15"/>
+    <sheet name="Switch" sheetId="12" r:id="rId16"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="247">
   <si>
     <t>Name:</t>
   </si>
@@ -221,9 +222,6 @@
   </si>
   <si>
     <t>Map entrance to 1F</t>
-  </si>
-  <si>
-    <t>Map entrance to 1F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -241,10 +239,6 @@
     <t>StorageShack</t>
   </si>
   <si>
-    <t>StorageShack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Map entrance</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -826,6 +820,167 @@
   </si>
   <si>
     <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001: DayTime, 008: TownLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30x25</t>
+  </si>
+  <si>
+    <t>Exterior</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Town_lv1-1stNight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>守衛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>劇情,走位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-村長家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-鐵匠鋪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-教堂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-PUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OfficerHouse-1stNight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17x18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-Mr. Laurance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家設隱形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-守衛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>燈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蠟燭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-對話用Dummy玩家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防止玩家出門</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>休息點</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -869,7 +1024,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,6 +1043,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1360,7 @@
     <col min="3" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="13.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="37.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1210,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,7 +1401,7 @@
         <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>51</v>
@@ -1257,30 +1415,33 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>43</v>
@@ -1294,6 +1455,156 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="18" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -1316,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1324,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,7 +1643,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1349,7 +1660,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>50</v>
@@ -1363,13 +1674,13 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1377,13 +1688,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>27</v>
@@ -1394,7 +1705,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>35</v>
@@ -1411,16 +1722,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1428,16 +1739,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1445,16 +1756,16 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1462,16 +1773,16 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1479,7 +1790,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>32</v>
@@ -1488,7 +1799,7 @@
         <v>44</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1496,10 +1807,10 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
@@ -1514,7 +1825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -1537,7 +1848,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1545,7 +1856,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1553,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1570,7 +1881,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>50</v>
@@ -1584,16 +1895,16 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1603,10 +1914,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>39</v>
@@ -1622,7 +1933,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>45</v>
@@ -1631,7 +1942,7 @@
         <v>39</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -1641,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -1661,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,7 +1988,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,7 +2005,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -1708,10 +2019,10 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
@@ -1725,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>38</v>
@@ -1742,7 +2053,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>41</v>
@@ -1756,16 +2067,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +2085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -1795,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1803,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1811,7 +2122,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1828,7 +2139,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>50</v>
@@ -1842,13 +2153,13 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>26</v>
@@ -1859,13 +2170,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>26</v>
@@ -1876,19 +2187,19 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,16 +2207,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1914,7 +2225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -1935,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1951,7 +2262,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1968,7 +2279,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>50</v>
@@ -1982,17 +2293,17 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2002,7 +2313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -2018,90 +2329,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2114,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2132,7 +2443,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2140,7 +2451,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2148,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2165,7 +2476,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>50</v>
@@ -2179,16 +2490,16 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2196,16 +2507,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2213,33 +2524,33 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B9" t="s">
         <v>203</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2253,7 +2564,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2275,7 +2586,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2283,7 +2594,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2300,7 +2611,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -2314,13 +2625,13 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>27</v>
@@ -2334,17 +2645,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="3"/>
-    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="6"/>
+    <col min="5" max="5" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2352,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2360,7 +2672,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2368,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,14 +2690,14 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>67</v>
+      <c r="E5" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -2399,16 +2711,283 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>219</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="20.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>227</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F8" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>245</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2417,7 +2996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -2439,7 +3018,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2472,7 +3051,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
         <v>50</v>
@@ -2486,13 +3065,13 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>27</v>
@@ -2503,13 +3082,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>27</v>
@@ -2520,13 +3099,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>27</v>
@@ -2537,7 +3116,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>32</v>
@@ -2554,16 +3133,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2571,13 +3150,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2585,16 +3164,16 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" t="s">
         <v>74</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2602,33 +3181,33 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="F14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2636,13 +3215,13 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>27</v>
@@ -2654,7 +3233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -2674,7 +3253,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,7 +3269,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,10 +3286,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
         <v>52</v>
@@ -2721,10 +3300,10 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>32</v>
@@ -2739,10 +3318,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>43</v>
@@ -2758,7 +3337,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -2781,7 +3360,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2797,7 +3376,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,10 +3393,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
         <v>52</v>
@@ -2828,10 +3407,10 @@
         <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>32</v>
@@ -2846,13 +3425,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -2862,7 +3441,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>32</v>
@@ -2881,7 +3460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -2902,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2935,10 +3514,10 @@
         <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" t="s">
         <v>52</v>
@@ -2952,7 +3531,7 @@
         <v>23</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>31</v>
@@ -2966,166 +3545,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="18" style="2" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Add UpgradeTownHall1 quest in Office house -Add wood and stone harvest point -Add self customized character in Pub
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="Town_lv1" sheetId="3" r:id="rId3"/>
     <sheet name="Town_lv1-1stNight" sheetId="16" r:id="rId4"/>
     <sheet name="OfficerHouse-1stNight" sheetId="4" r:id="rId5"/>
-    <sheet name="MinatoPort" sheetId="5" r:id="rId6"/>
-    <sheet name="MinatoWeaponShop" sheetId="6" r:id="rId7"/>
+    <sheet name="Blacksmith_lv1" sheetId="5" r:id="rId6"/>
+    <sheet name="PUB_lv1" sheetId="6" r:id="rId7"/>
     <sheet name="MinatoInn" sheetId="7" r:id="rId8"/>
     <sheet name="MinatoItemShop" sheetId="8" r:id="rId9"/>
     <sheet name="WorldMap1" sheetId="9" r:id="rId10"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="243">
   <si>
     <t>Name:</t>
   </si>
@@ -98,9 +98,6 @@
     <t>EV009</t>
   </si>
   <si>
-    <t>EV010</t>
-  </si>
-  <si>
     <t>EV001</t>
   </si>
   <si>
@@ -170,80 +167,779 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interior</t>
+  </si>
+  <si>
+    <t>17x13</t>
+  </si>
+  <si>
+    <t>17x13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Variable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map entrance to 1F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map entrance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapEntrance</t>
+  </si>
+  <si>
+    <t>MapEntrance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapEntrance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001: Winter join the team</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0002: Allow to use boat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinatoInn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老闆娘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinatoItemShop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>道具店老闆娘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WorldMap1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40x30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Field</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>村莊入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>037</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遺跡入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MinatoPort入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>船: 測試</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cave of Demon入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>031</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoD_F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40x40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dungeon</t>
+  </si>
+  <si>
+    <t>Dungeon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關卡測試</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地城入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地下出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寶箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-道具開門測試</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0003: Opened cave door </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寶箱-Cave of Demon Key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004:Open cave gate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>028</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖刺陷阱1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖刺陷阱2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CoD_F2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>40x20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女神像前傳送點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 大叔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0005:Get airship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0003: Opened cave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004: Open cave gate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0005: Get airship</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0006: EnterTheCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Winter加入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>問村長四次後設為on並顯示Quest complete: Use the boat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cave of Demon key在道具欄裡第二道門開啟後設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用Cave of Demon key開啟Cave of Demon中第一道門後設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟Cave of Demon第二層大叔對話後設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回答LavaCave的守護石像security code問題後設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擊敗Morris和地獄犬後設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dungeon1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖出入口</t>
+  </si>
+  <si>
+    <t>地圖出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LavaCave出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石板顯示Security code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LavaCave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>029</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>守護石像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0003: SecurityCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0006:EnterTheCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boss NPC - 邪惡祭司Morris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0007: DefeatMorris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0008: GameEnd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0007: DefeatMorris 0008: GameEnd </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoodKingRoom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - King</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0007:DefeatMorris</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0009: Iryss join the team</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Iryss加入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0022:PMemberOn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>設為On後更新四個variable記錄隊伍位置1,2,3,4,5,6,7,8使用的Actor可用於交換隊伍成員</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Introduction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>捲動字幕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starting point</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MystForst01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17x20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exterior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解除Starting point的透明效果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主角起始點, 操作說明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - Bandit埋伏點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Town_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exterior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30x25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傳送點-去Town_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001: DayTime, 008: TownLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30x25</t>
+  </si>
+  <si>
+    <t>Exterior</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>Town_lv1-1stNight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>守衛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>劇情,走位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-村長家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-鐵匠鋪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-教堂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>門-PUB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OfficerHouse-1stNight</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17x18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-Mr. Laurance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩家設隱形</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-守衛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>燈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>蠟燭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC-對話用Dummy玩家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>011</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>027</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防止玩家出門</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>休息點</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blacksmith</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Interior</t>
-  </si>
-  <si>
-    <t>17x13</t>
-  </si>
-  <si>
-    <t>17x13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>Switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Variable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map entrance to 1F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Door</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鐵匠店入口</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>008</t>
-  </si>
-  <si>
-    <t>008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StorageShack</t>
-  </si>
-  <si>
-    <t>Map entrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV003</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -251,736 +947,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Weapon shop entrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MapEntrance</t>
-  </si>
-  <si>
-    <t>MapEntrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MapEntrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Inn entrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item shop entrance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>014</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Winter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001: Winter join the team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC - 史密斯船長</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0002: Allow to use boat</t>
-  </si>
-  <si>
-    <t>0002: Allow to use boat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV009</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0002: Allow to use boat 0007:DefeatMorris 0021:BorrowShip</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>設定船出現位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出海位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MinatoWeaponShop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>武器店老闆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MinatoInn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>老闆娘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>提示</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MinatoItemShop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>道具店老闆娘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WorldMap1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>40x30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Field</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>村莊入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>037</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>遺跡入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MinatoPort入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>020</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>017</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>018</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>船: 測試</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cave of Demon入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>031</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>027</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoD_F1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>40x40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dungeon</t>
-  </si>
-  <si>
-    <t>Dungeon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>關卡測試</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>021</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>025</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>032</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地城入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地下出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>寶箱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>022</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門-道具開門測試</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0003: Opened cave door </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>寶箱-Cave of Demon Key</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0004:Open cave gate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>028</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>尖刺陷阱1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>尖刺陷阱2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoD_F2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>40x20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>030</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>女神像前傳送點</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC - 大叔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0005:Get airship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0003: Opened cave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0004: Open cave gate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0005: Get airship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0006: EnterTheCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Winter加入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>問村長四次後設為on並顯示Quest complete: Use the boat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cave of Demon key在道具欄裡第二道門開啟後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用Cave of Demon key開啟Cave of Demon中第一道門後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>跟Cave of Demon第二層大叔對話後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回答LavaCave的守護石像security code問題後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>擊敗Morris和地獄犬後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dungeon1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地圖出入口</t>
-  </si>
-  <si>
-    <t>地圖出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LavaCave出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>石板顯示Security code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LavaCave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>029</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>守護石像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>033</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0003: SecurityCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0006:EnterTheCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss NPC - 邪惡祭司Morris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0007: DefeatMorris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0008: GameEnd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0007: DefeatMorris 0008: GameEnd </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GoodKingRoom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Interior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC - King</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0007:DefeatMorris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0009: Iryss join the team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iryss加入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0022:PMemberOn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>設為On後更新四個variable記錄隊伍位置1,2,3,4,5,6,7,8使用的Actor可用於交換隊伍成員</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Introduction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>捲動字幕</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Start</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Starting point</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MystForst01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17x20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exterior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>解除Starting point的透明效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主角起始點, 操作說明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>019</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC - Bandit埋伏點</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Self switch A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Self switch A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Town_lv1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exterior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30x25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>傳送點-去Town_lv1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0001: DayTime, 008: TownLevel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30x25</t>
-  </si>
-  <si>
-    <t>Exterior</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>Town_lv1-1stNight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>守衛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>劇情,走位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門-村長家</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門-鐵匠鋪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門-教堂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>門-PUB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OfficerHouse-1stNight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17x18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC-Mr. Laurance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>玩家設隱形</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC-守衛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>燈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>蠟燭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>012</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC-對話用Dummy玩家</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>010</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV007</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>防止玩家出門</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>017</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>休息點</t>
+    <t>NPC-Blacksmith 鐵匠鋪商店</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUB_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20x20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUB入口1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUB入口2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1350,7 +1337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -1368,7 +1355,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1395,56 +1382,56 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1461,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1490,7 +1477,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1501,36 +1488,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1538,16 +1525,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1555,16 +1542,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1572,30 +1559,30 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1635,7 +1622,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1654,33 +1641,33 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,16 +1675,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1705,16 +1692,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1722,16 +1709,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1739,16 +1726,16 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1756,16 +1743,16 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1773,16 +1760,16 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1790,16 +1777,16 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1807,16 +1794,16 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1848,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1856,7 +1843,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1864,7 +1851,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1875,36 +1862,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -1914,16 +1901,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -1933,16 +1920,16 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="G8" s="5"/>
     </row>
@@ -1972,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,7 +1975,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1999,36 +1986,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2036,16 +2023,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2053,30 +2040,30 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2106,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2114,7 +2101,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2122,7 +2109,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2133,36 +2120,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2170,16 +2157,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2187,19 +2174,19 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2207,16 +2194,16 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2246,7 +2233,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2254,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2262,7 +2249,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2273,37 +2260,37 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2329,90 +2316,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2443,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2451,7 +2438,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2459,7 +2446,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2470,36 +2457,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2507,16 +2494,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2524,33 +2511,33 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2578,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2586,7 +2573,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2594,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2605,36 +2592,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2664,7 +2651,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2672,7 +2659,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2680,7 +2667,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2691,112 +2678,112 @@
         <v>11</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="B10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2811,7 +2798,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2827,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2835,7 +2822,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2843,7 +2830,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2854,140 +2841,140 @@
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="F8" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="B9" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B10" t="s">
-        <v>237</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>238</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" t="s">
         <v>218</v>
       </c>
-      <c r="B11" t="s">
-        <v>239</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2998,15 +2985,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="23.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="51.140625" customWidth="1"/>
@@ -3018,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3026,7 +3013,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3034,7 +3021,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3045,186 +3032,67 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>50</v>
-      </c>
-      <c r="G5" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>228</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>231</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>61</v>
+        <v>233</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>27</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>235</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>238</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>232</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>27</v>
+        <v>236</v>
+      </c>
+      <c r="F8" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3237,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3253,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3261,7 +3129,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3269,7 +3137,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3280,36 +3148,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>241</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -3318,16 +3186,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>242</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>220</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -3360,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3368,7 +3236,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3376,7 +3244,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3387,36 +3255,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -3425,13 +3293,13 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -3441,17 +3309,17 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -3481,7 +3349,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3489,7 +3357,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3497,7 +3365,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3508,36 +3376,36 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3545,16 +3413,16 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add church_lv2 map -Add Madlyn in the town_lv2 map -Add father -Add caravian in the town_lv2 map
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Town_lv2" sheetId="8" r:id="rId9"/>
     <sheet name="TownHall_lv2" sheetId="9" r:id="rId10"/>
     <sheet name="Blacksmith_lv2" sheetId="10" r:id="rId11"/>
-    <sheet name="HerosHut_lv1" sheetId="11" r:id="rId12"/>
-    <sheet name="Dungeon1" sheetId="13" r:id="rId13"/>
-    <sheet name="LavaCave" sheetId="14" r:id="rId14"/>
+    <sheet name="HerosHutMap_lv1" sheetId="11" r:id="rId12"/>
+    <sheet name="HerosHut_lv1" sheetId="13" r:id="rId13"/>
+    <sheet name="Church_lv2" sheetId="14" r:id="rId14"/>
     <sheet name="GoodKingsRoom" sheetId="15" r:id="rId15"/>
     <sheet name="Switch" sheetId="12" r:id="rId16"/>
     <sheet name="Variables" sheetId="17" r:id="rId17"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="337">
   <si>
     <t>Name:</t>
   </si>
@@ -47,10 +47,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>30x20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TileSet:</t>
   </si>
   <si>
@@ -122,10 +118,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>019</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -137,10 +129,6 @@
     <t>007</t>
   </si>
   <si>
-    <t>013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>014</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -211,10 +199,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>014</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0001: Winter join the team</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,10 +215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>40x30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>021</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,9 +231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dungeon</t>
-  </si>
-  <si>
     <t>022</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -314,74 +291,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Dungeon1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>地圖出入口</t>
   </si>
   <si>
-    <t>地圖出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LavaCave出入口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>EV004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>石板顯示Security code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>011</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LavaCave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>029</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>守護石像</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>033</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0003: SecurityCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0006:EnterTheCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Boss NPC - 邪惡祭司Morris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0007: DefeatMorris</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0008: GameEnd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">0007: DefeatMorris 0008: GameEnd </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1188,19 +1105,202 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Exterior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出入口2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出入口1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0002: TownHallLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主角小屋出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://maou.audio/help-filetype/</t>
+  </si>
+  <si>
+    <t>主角小屋簡介事件觸發</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HerosHutMap_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>出入口1</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
     <t>HerosHut_lv1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Exterior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出入口2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出入口1</t>
+    <t>17x13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>床-休息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>書</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0024:ASmallHutComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Harvesting point - wood</t>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV009</t>
+  </si>
+  <si>
+    <t>EV010</t>
+  </si>
+  <si>
+    <t>EV011</t>
+  </si>
+  <si>
+    <t>EV012</t>
+  </si>
+  <si>
+    <t>NPC - 馬車帳棚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 馬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 商人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - Madlyn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Church_lv2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17x25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Interior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 神父</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1208,15 +1308,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>013</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0002: TownHallLevel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主角小屋出入口</t>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1620,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,75 +1724,75 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1727,7 +1823,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1735,149 +1831,149 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="11" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1906,10 +2002,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="B1" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1917,7 +2013,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2"/>
@@ -1925,10 +2021,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3"/>
@@ -1941,39 +2037,39 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6"/>
@@ -1981,39 +2077,39 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="G8"/>
     </row>
@@ -2028,10 +2124,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2040,7 +2136,7 @@
     <col min="3" max="3" width="9.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2049,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2057,100 +2153,131 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>306</v>
+        <v>284</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" t="s">
+        <v>309</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>311</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2160,10 +2287,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2178,7 +2305,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>298</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2186,103 +2313,83 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>295</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>301</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>296</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>304</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>302</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>305</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>306</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2293,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2320,109 +2427,140 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>329</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>330</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>331</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>88</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>93</v>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2452,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2460,56 +2598,56 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2535,90 +2673,90 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2643,228 +2781,228 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
     </row>
     <row r="33" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2881,7 +3019,16 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2909,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2917,106 +3064,106 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3030,7 +3177,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3047,7 +3194,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3055,179 +3202,179 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="G14" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3258,7 +3405,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3266,131 +3413,131 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3418,10 +3565,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3429,159 +3576,159 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" t="s">
         <v>139</v>
       </c>
-      <c r="B11" t="s">
-        <v>160</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3610,10 +3757,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3624,7 +3771,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3632,10 +3779,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3648,63 +3795,63 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="10" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3765,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3773,86 +3920,86 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3882,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3890,158 +4037,158 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -4052,17 +4199,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
     <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4071,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4083,7 +4230,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4092,10 +4239,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4110,162 +4257,217 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="F8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
       <c r="E11" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+        <v>178</v>
+      </c>
+      <c r="B12" t="s">
+        <v>317</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>318</v>
+      </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B15" t="s">
+        <v>321</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" t="s">
+        <v>324</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>315</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Rename guard to Bruce. Add events to Bruce - Add new actor Hans. Add events - Update SwitchVariableConf.xlsx
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="464">
   <si>
     <t>Name:</t>
   </si>
@@ -199,14 +199,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0001: Winter join the team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0002: Allow to use boat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>003</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -247,61 +239,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0003: Opened cave</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0004: Open cave gate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0005: Get airship</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0006: EnterTheCode</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Winter加入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>問村長四次後設為on並顯示Quest complete: Use the boat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cave of Demon key在道具欄裡第二道門開啟後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用Cave of Demon key開啟Cave of Demon中第一道門後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>跟Cave of Demon第二層大叔對話後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回答LavaCave的守護石像security code問題後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>擊敗Morris和地獄犬後設為ON</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>地圖出入口</t>
   </si>
   <si>
-    <t>0007: DefeatMorris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0008: GameEnd</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GoodKingRoom</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -318,22 +258,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0009: Iryss join the team</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iryss加入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0022:PMemberOn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>設為On後更新四個variable記錄隊伍位置1,2,3,4,5,6,7,8使用的Actor可用於交換隊伍成員</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Introduction</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -374,10 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>解除Starting point的透明效果</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>主角起始點, 操作說明</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -391,10 +311,6 @@
   </si>
   <si>
     <t>008</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Self switch A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1308,11 +1224,520 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>016</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>012</t>
+    <t>解除Starting point的透明效果,設隊伍人數為1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self switch A, 0021:PMemberNumber</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMember8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0005:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0006:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0007:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0008:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0009: </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0010:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0011:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>41:</t>
+  </si>
+  <si>
+    <t>42:</t>
+  </si>
+  <si>
+    <t>43:</t>
+  </si>
+  <si>
+    <t>44:</t>
+  </si>
+  <si>
+    <t>45:</t>
+  </si>
+  <si>
+    <t>46:</t>
+  </si>
+  <si>
+    <t>47:</t>
+  </si>
+  <si>
+    <t>48:</t>
+  </si>
+  <si>
+    <t>49:</t>
+  </si>
+  <si>
+    <t>50:</t>
+  </si>
+  <si>
+    <t>51:</t>
+  </si>
+  <si>
+    <t>52:</t>
+  </si>
+  <si>
+    <t>53:</t>
+  </si>
+  <si>
+    <t>54:</t>
+  </si>
+  <si>
+    <t>55:</t>
+  </si>
+  <si>
+    <t>56:</t>
+  </si>
+  <si>
+    <t>57:</t>
+  </si>
+  <si>
+    <t>58:</t>
+  </si>
+  <si>
+    <t>59:</t>
+  </si>
+  <si>
+    <t>60:</t>
+  </si>
+  <si>
+    <t>61:</t>
+  </si>
+  <si>
+    <t>62:</t>
+  </si>
+  <si>
+    <t>63:</t>
+  </si>
+  <si>
+    <t>64:</t>
+  </si>
+  <si>
+    <t>65:</t>
+  </si>
+  <si>
+    <t>66:</t>
+  </si>
+  <si>
+    <t>67:</t>
+  </si>
+  <si>
+    <t>68:</t>
+  </si>
+  <si>
+    <t>69:</t>
+  </si>
+  <si>
+    <t>70:</t>
+  </si>
+  <si>
+    <t>71:</t>
+  </si>
+  <si>
+    <t>72:</t>
+  </si>
+  <si>
+    <t>73:</t>
+  </si>
+  <si>
+    <t>74:</t>
+  </si>
+  <si>
+    <t>75:</t>
+  </si>
+  <si>
+    <t>76:</t>
+  </si>
+  <si>
+    <t>77:</t>
+  </si>
+  <si>
+    <t>78:</t>
+  </si>
+  <si>
+    <t>79:</t>
+  </si>
+  <si>
+    <t>80:</t>
+  </si>
+  <si>
+    <t>81:</t>
+  </si>
+  <si>
+    <t>82:</t>
+  </si>
+  <si>
+    <t>83:</t>
+  </si>
+  <si>
+    <t>84:</t>
+  </si>
+  <si>
+    <t>85:</t>
+  </si>
+  <si>
+    <t>86:</t>
+  </si>
+  <si>
+    <t>87:</t>
+  </si>
+  <si>
+    <t>88:</t>
+  </si>
+  <si>
+    <t>89:</t>
+  </si>
+  <si>
+    <t>90:</t>
+  </si>
+  <si>
+    <t>91:</t>
+  </si>
+  <si>
+    <t>92:</t>
+  </si>
+  <si>
+    <t>93:</t>
+  </si>
+  <si>
+    <t>94:</t>
+  </si>
+  <si>
+    <t>95:</t>
+  </si>
+  <si>
+    <t>96:</t>
+  </si>
+  <si>
+    <t>97:</t>
+  </si>
+  <si>
+    <t>98:</t>
+  </si>
+  <si>
+    <t>99:</t>
+  </si>
+  <si>
+    <t>100:</t>
+  </si>
+  <si>
+    <t>0012:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0013:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0014:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0015:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0016:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0017:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0018:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0019:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0020:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0029:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0030:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0031:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0032:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0033:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0034:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0035:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0036:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0037:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0038:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0039:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0040:</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0021:TownHallUpgrade1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0022:TownHallUpg1Complete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0023:ASmallHut</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0024:ASmallHutComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0025:FirstCaravan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一隊商隊抵達</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升級TownHall一級任務用於OfficerHouse_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成 升級TownHall一級任務用於OfficerHouse_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>領取勇者小屋用於TownHall_lv2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>看完勇者小屋簡介動畫HerosHutMap_lv1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0026:MeetMadlyn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001: MadlynAvailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0002: BruceAvailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>當Madlyn離隊時設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>當Bruce離隊時設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0038</t>
+  </si>
+  <si>
+    <t>0039</t>
+  </si>
+  <si>
+    <t>0040</t>
+  </si>
+  <si>
+    <t>0041</t>
+  </si>
+  <si>
+    <t>0042</t>
+  </si>
+  <si>
+    <t>0043</t>
+  </si>
+  <si>
+    <t>0044</t>
+  </si>
+  <si>
+    <t>0045</t>
+  </si>
+  <si>
+    <t>0046</t>
+  </si>
+  <si>
+    <t>0047</t>
+  </si>
+  <si>
+    <t>0048</t>
+  </si>
+  <si>
+    <t>0049</t>
+  </si>
+  <si>
+    <t>0050</t>
+  </si>
+  <si>
+    <t>0051</t>
+  </si>
+  <si>
+    <t>0052</t>
+  </si>
+  <si>
+    <t>0053</t>
+  </si>
+  <si>
+    <t>0054</t>
+  </si>
+  <si>
+    <t>0055</t>
+  </si>
+  <si>
+    <t>0056</t>
+  </si>
+  <si>
+    <t>0057</t>
+  </si>
+  <si>
+    <t>0058</t>
+  </si>
+  <si>
+    <t>0059</t>
+  </si>
+  <si>
+    <t>0060</t>
+  </si>
+  <si>
+    <t>MadlynRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BruceRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madly友好度, 初始值為100, 最大值100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bruce友好度,初始值為50,最大值100 每一次成功冒險+10 每一次死亡結算-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Madlyn初抵達村莊時對話完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0027:MeetBruce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pub初次和Bruce對話完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HansRelation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0028:MeetHans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pub初次和Hans對話完成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0003: HansAvailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>當Hans離隊時設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hans友好度,初始值為50,最大值100每一次成功冒險+10 每一次死亡結算-20</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1716,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,30 +2188,30 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
@@ -1823,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1831,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,7 +2264,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1870,7 +2295,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>32</v>
@@ -1884,7 +2309,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>32</v>
@@ -1898,7 +2323,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
@@ -1912,25 +2337,25 @@
         <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="11" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>31</v>
@@ -1947,16 +2372,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1964,16 +2389,16 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2002,10 +2427,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B1" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2024,7 +2449,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3"/>
@@ -2063,10 +2488,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>41</v>
@@ -2077,10 +2502,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
@@ -2089,27 +2514,27 @@
         <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="G8"/>
     </row>
@@ -2145,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2153,7 +2578,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2161,7 +2586,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2192,20 +2617,20 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2213,20 +2638,20 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2234,49 +2659,49 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="B9" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -2305,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2313,7 +2738,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,7 +2746,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2352,13 +2777,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
@@ -2369,13 +2794,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2383,13 +2808,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -2400,10 +2825,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2419,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2427,7 +2852,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2435,7 +2860,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2466,13 +2891,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
@@ -2483,13 +2908,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2497,16 +2922,16 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -2516,16 +2941,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -2534,33 +2959,16 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -2590,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2606,7 +3014,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2637,7 +3045,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>41</v>
@@ -2647,7 +3055,7 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="6" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2659,7 +3067,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -2673,90 +3081,543 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>424</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>63</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>425</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>64</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>59</v>
+        <v>461</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>66</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>65</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>68</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>69</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>78</v>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="6" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="6" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="6" t="s">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -2767,242 +3628,399 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" customWidth="1"/>
+    <col min="3" max="3" width="83.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>251</v>
+        <v>230</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>252</v>
+        <v>231</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>253</v>
+        <v>232</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>254</v>
+        <v>233</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>255</v>
+        <v>234</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>256</v>
+        <v>235</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>257</v>
+        <v>236</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" s="13" customFormat="1" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>264</v>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>431</v>
+      </c>
+      <c r="B42" t="s">
+        <v>451</v>
+      </c>
+      <c r="C42" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>432</v>
+      </c>
+      <c r="B43" t="s">
+        <v>452</v>
+      </c>
+      <c r="C43" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="B44" t="s">
+        <v>458</v>
+      </c>
+      <c r="C44" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3025,7 +4043,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3039,7 +4057,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3056,7 +4074,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3064,7 +4082,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3072,7 +4090,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3103,16 +4121,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>314</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>97</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3120,16 +4138,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3137,33 +4155,33 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B9" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3194,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3202,7 +4220,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3210,7 +4228,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3241,13 +4259,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -3255,126 +4273,126 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="G14" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3405,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3413,7 +4431,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3421,7 +4439,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3452,13 +4470,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>22</v>
@@ -3466,44 +4484,44 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>30</v>
@@ -3514,13 +4532,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
@@ -3528,10 +4546,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>25</v>
@@ -3565,10 +4583,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3576,7 +4594,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3615,7 +4633,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>40</v>
@@ -3627,108 +4645,108 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="F8" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>138</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
         <v>118</v>
       </c>
-      <c r="B11" t="s">
-        <v>139</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -3757,10 +4775,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -3771,7 +4789,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -3821,13 +4839,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>23</v>
@@ -3835,10 +4853,10 @@
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>41</v>
@@ -3848,10 +4866,10 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="10" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3912,7 +4930,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3928,7 +4946,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3959,47 +4977,47 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -4029,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4037,7 +5055,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4045,7 +5063,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4065,7 +5083,7 @@
         <v>44</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -4076,7 +5094,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>30</v>
@@ -4094,10 +5112,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>25</v>
@@ -4112,13 +5130,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4126,13 +5144,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4140,13 +5158,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4154,13 +5172,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4168,13 +5186,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4182,13 +5200,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -4201,7 +5219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4218,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4230,7 +5248,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4242,7 +5260,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -4283,13 +5301,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -4298,171 +5316,171 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="F8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
       <c r="E11" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="B12" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
       <c r="B14" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
       <c r="B15" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="B16" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Update map MystForestA with map events - Update common event with MystForestA map events - Add Lyndiss event in MystForestA
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="HerosHutMap_lv1" sheetId="11" r:id="rId12"/>
     <sheet name="HerosHut_lv1" sheetId="13" r:id="rId13"/>
     <sheet name="Church_lv2" sheetId="14" r:id="rId14"/>
-    <sheet name="GoodKingsRoom" sheetId="15" r:id="rId15"/>
+    <sheet name="MystForestA" sheetId="15" r:id="rId15"/>
     <sheet name="Switch" sheetId="12" r:id="rId16"/>
     <sheet name="Variables" sheetId="17" r:id="rId17"/>
     <sheet name="Sheet2" sheetId="18" r:id="rId18"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="534">
   <si>
     <t>Name:</t>
   </si>
@@ -180,10 +180,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MapEntrance</t>
   </si>
   <si>
@@ -242,19 +238,7 @@
     <t>地圖出入口</t>
   </si>
   <si>
-    <t>GoodKingRoom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Interior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC - King</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0007:DefeatMorris</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1264,10 +1248,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0004:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0005:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1296,63 +1276,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>41:</t>
-  </si>
-  <si>
-    <t>42:</t>
-  </si>
-  <si>
-    <t>43:</t>
-  </si>
-  <si>
-    <t>44:</t>
-  </si>
-  <si>
-    <t>45:</t>
-  </si>
-  <si>
-    <t>46:</t>
-  </si>
-  <si>
-    <t>47:</t>
-  </si>
-  <si>
-    <t>48:</t>
-  </si>
-  <si>
-    <t>49:</t>
-  </si>
-  <si>
-    <t>50:</t>
-  </si>
-  <si>
-    <t>51:</t>
-  </si>
-  <si>
-    <t>52:</t>
-  </si>
-  <si>
-    <t>53:</t>
-  </si>
-  <si>
-    <t>54:</t>
-  </si>
-  <si>
-    <t>55:</t>
-  </si>
-  <si>
-    <t>56:</t>
-  </si>
-  <si>
-    <t>57:</t>
-  </si>
-  <si>
-    <t>58:</t>
-  </si>
-  <si>
-    <t>59:</t>
-  </si>
-  <si>
     <t>60:</t>
   </si>
   <si>
@@ -1512,10 +1435,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0029:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0030:</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1536,30 +1455,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0035:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0036:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0037:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0038:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0039:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0040:</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0021:TownHallUpgrade1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1738,6 +1633,400 @@
   </si>
   <si>
     <t>Hans友好度,初始值為50,最大值100每一次成功冒險+10 每一次死亡結算-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0004: LyndissAvailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>當Lyndiss離隊時設為ON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0029:MeetLyndiss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0035:MystForestAComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0036:MystForestBComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0037:MystForestCComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapEventPattern</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>決定地城地圖事件變數: 1-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0038:CaveAComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0039:CaveBComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0040:CaveCComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0041:DungeonAComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0042:DungeonBComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0043:DungeonCComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0044:ABVillageAComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0045:ABVillageBComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0046:ABVillageCComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0047:MForestA_EV010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0048:MForestA_EV011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0049:MForestA_EV012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0050:MForestA_EV013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0051:MForestA_EV014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0052:MForestA_EV015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0053:MForestA_EV016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0054:MForestA_EV017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0055:MForestA_EV018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MistForestA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30x40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exterior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瀑布效果1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瀑布效果2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瀑布效果3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瀑布效果4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV013</t>
+  </si>
+  <si>
+    <t>EV014</t>
+  </si>
+  <si>
+    <t>EV015</t>
+  </si>
+  <si>
+    <t>EV016</t>
+  </si>
+  <si>
+    <t>EV017</t>
+  </si>
+  <si>
+    <t>EV018</t>
+  </si>
+  <si>
+    <t>EV019</t>
+  </si>
+  <si>
+    <t>EV020</t>
+  </si>
+  <si>
+    <t>EV021</t>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lyndiss劇情觸發</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Self Switch A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 狼 Lyndiss劇情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - Lyndiss Lyndiss劇情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 狼 Lyndiss劇情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004:MapEventPattern</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0047:MForestA_EV010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寶箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資源事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖參數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0048:MForestA_EV011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0049:MForestA_EV012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0050:MForestA_EV013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0051:MForestA_EV014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0052:MForestA_EV015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0053:MForestA_EV016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0054:MForestA_EV017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0055:MForestA_EV018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0056:MForestA_EV019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0057:MForestA_EV020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0058:MForestA_EV021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV022</t>
+  </si>
+  <si>
+    <t>0059:MForestA_EV022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0059:MForestA_EV022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterEventRand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChestEventRand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShrineEventRand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個變數用來決定每次Monster Event碰到的敵人隊伍: 1-5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個變數用來決定每次Chest Event開到的寶物組合: 1-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個變數用來決定每次Shrine造成的隊伍buff/debuff: 1-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LootEventRand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個變數用來決定每次固定寶箱開到的寶物組合: 1-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TrapEventRand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>這個變數用來決定地圖陷阱:1-10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1761,12 +2050,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1781,7 +2076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1820,6 +2115,16 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2141,7 +2446,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2174,7 +2479,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>37</v>
@@ -2188,30 +2493,30 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
@@ -2248,7 +2553,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2256,7 +2561,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2264,7 +2569,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2281,7 +2586,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>36</v>
@@ -2295,7 +2600,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>32</v>
@@ -2309,7 +2614,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>32</v>
@@ -2323,7 +2628,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
@@ -2337,25 +2642,25 @@
         <v>13</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>31</v>
@@ -2372,16 +2677,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2389,16 +2694,16 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2427,10 +2732,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2449,7 +2754,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3"/>
@@ -2474,7 +2779,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -2488,10 +2793,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>41</v>
@@ -2502,39 +2807,39 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G8"/>
     </row>
@@ -2570,7 +2875,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2578,7 +2883,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2586,7 +2891,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2603,7 +2908,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>36</v>
@@ -2617,20 +2922,20 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2638,20 +2943,20 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2659,49 +2964,49 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B9" t="s">
         <v>268</v>
       </c>
-      <c r="B9" t="s">
-        <v>272</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B10" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -2730,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2738,7 +3043,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2746,7 +3051,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2763,7 +3068,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -2777,13 +3082,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
@@ -2794,13 +3099,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2808,13 +3113,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2844,7 +3149,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2852,7 +3157,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2860,7 +3165,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2877,7 +3182,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>36</v>
@@ -2891,13 +3196,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>22</v>
@@ -2908,13 +3213,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2922,16 +3227,16 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -2941,16 +3246,16 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -2959,16 +3264,16 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -2979,18 +3284,19 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="13"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="5"/>
+    <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2998,7 +3304,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3006,7 +3312,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3014,7 +3320,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3031,7 +3337,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>36</v>
@@ -3045,17 +3351,361 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>462</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>277</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="6" t="s">
-        <v>61</v>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>468</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>481</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>482</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>484</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>479</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>486</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>487</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>509</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+    </row>
+    <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>493</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>490</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>510</v>
+      </c>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>503</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>511</v>
+      </c>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>504</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>505</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>513</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>472</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>479</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>508</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>514</v>
+      </c>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>480</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>502</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>489</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>491</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>476</v>
+      </c>
+      <c r="B24" t="s">
+        <v>497</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>469</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>477</v>
+      </c>
+      <c r="B25" t="s">
+        <v>497</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>478</v>
+      </c>
+      <c r="B26" t="s">
+        <v>500</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>521</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>522</v>
       </c>
     </row>
   </sheetData>
@@ -3069,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3081,543 +3731,546 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>425</v>
+        <v>394</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>427</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>461</v>
+        <v>430</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>462</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>324</v>
+        <v>433</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>413</v>
+        <v>382</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>419</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>420</v>
+        <v>389</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>421</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>422</v>
+        <v>391</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>417</v>
+        <v>386</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>418</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>423</v>
+        <v>392</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>455</v>
+        <v>424</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>456</v>
+        <v>425</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>457</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>459</v>
+        <v>428</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>460</v>
+        <v>429</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>401</v>
+        <v>435</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>402</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>403</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>404</v>
+        <v>379</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>405</v>
+        <v>380</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>407</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>408</v>
+        <v>437</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>409</v>
+        <v>438</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>410</v>
+        <v>441</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>411</v>
+        <v>442</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>412</v>
+        <v>443</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>332</v>
+        <v>444</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>333</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>334</v>
+        <v>446</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>335</v>
+        <v>447</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>336</v>
+        <v>448</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>337</v>
+        <v>449</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>338</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>339</v>
+        <v>451</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>340</v>
+        <v>452</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>341</v>
+        <v>453</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>342</v>
+        <v>454</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>343</v>
+        <v>455</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>344</v>
+        <v>456</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>345</v>
+        <v>457</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>346</v>
+        <v>458</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>347</v>
+        <v>518</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>348</v>
+        <v>519</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>349</v>
+        <v>520</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>350</v>
+        <v>523</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -3631,7 +4284,7 @@
   <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3642,385 +4295,421 @@
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>210</v>
+        <v>206</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>212</v>
+        <v>208</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>213</v>
+        <v>209</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>526</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>214</v>
+        <v>210</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>530</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>215</v>
+        <v>211</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>532</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="35" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>431</v>
+        <v>400</v>
       </c>
       <c r="B42" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
       <c r="C42" t="s">
-        <v>453</v>
+        <v>422</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>432</v>
+        <v>401</v>
       </c>
       <c r="B43" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="C43" t="s">
-        <v>454</v>
+        <v>423</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>433</v>
+        <v>402</v>
       </c>
       <c r="B44" t="s">
-        <v>458</v>
+        <v>427</v>
       </c>
       <c r="C44" t="s">
-        <v>463</v>
+        <v>432</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>434</v>
+        <v>403</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>435</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>436</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>437</v>
+        <v>406</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>438</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>439</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>440</v>
+        <v>409</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>441</v>
+        <v>410</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>442</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>443</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>445</v>
+        <v>414</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>446</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>447</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>448</v>
+        <v>417</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>449</v>
+        <v>418</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>450</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -4043,7 +4732,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4074,7 +4763,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4082,7 +4771,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4090,7 +4779,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4107,7 +4796,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>36</v>
@@ -4121,16 +4810,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4138,16 +4827,16 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4155,33 +4844,33 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4212,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4220,7 +4909,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4228,7 +4917,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4245,7 +4934,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -4259,13 +4948,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -4273,126 +4962,126 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G14" t="s">
         <v>246</v>
-      </c>
-      <c r="B14" t="s">
-        <v>247</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G14" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4423,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4431,7 +5120,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4439,7 +5128,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4456,7 +5145,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -4470,13 +5159,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>22</v>
@@ -4484,44 +5173,44 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
         <v>95</v>
-      </c>
-      <c r="B9" t="s">
-        <v>99</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>30</v>
@@ -4532,13 +5221,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" t="s">
         <v>96</v>
       </c>
-      <c r="B10" t="s">
-        <v>100</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>30</v>
@@ -4546,10 +5235,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
         <v>97</v>
-      </c>
-      <c r="B11" t="s">
-        <v>101</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>25</v>
@@ -4583,10 +5272,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4594,7 +5283,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4619,7 +5308,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -4633,7 +5322,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>40</v>
@@ -4645,108 +5334,108 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4775,10 +5464,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -4789,7 +5478,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -4825,7 +5514,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -4839,13 +5528,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>23</v>
@@ -4853,10 +5542,10 @@
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>41</v>
@@ -4866,10 +5555,10 @@
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="10" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -4930,7 +5619,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4946,7 +5635,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4963,7 +5652,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -4977,47 +5666,47 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>131</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -5047,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -5055,7 +5744,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -5063,7 +5752,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -5080,10 +5769,10 @@
         <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -5094,7 +5783,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>30</v>
@@ -5112,10 +5801,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>25</v>
@@ -5130,13 +5819,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5144,13 +5833,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5158,13 +5847,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5172,13 +5861,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5186,13 +5875,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5200,13 +5889,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -5236,7 +5925,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -5248,7 +5937,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -5260,7 +5949,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -5287,7 +5976,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -5301,13 +5990,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>23</v>
@@ -5316,171 +6005,171 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B8" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>252</v>
-      </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" t="s">
         <v>291</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B15" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B16" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update MystForestB map. Add map event and map exit
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,17 @@
     <sheet name="HerosHut_lv1" sheetId="13" r:id="rId13"/>
     <sheet name="Church_lv2" sheetId="14" r:id="rId14"/>
     <sheet name="MystForestA" sheetId="15" r:id="rId15"/>
-    <sheet name="Switch" sheetId="12" r:id="rId16"/>
-    <sheet name="Variables" sheetId="17" r:id="rId17"/>
-    <sheet name="Sheet2" sheetId="18" r:id="rId18"/>
+    <sheet name="MystForestB" sheetId="19" r:id="rId16"/>
+    <sheet name="Switch" sheetId="12" r:id="rId17"/>
+    <sheet name="Variables" sheetId="17" r:id="rId18"/>
+    <sheet name="resource" sheetId="18" r:id="rId19"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="599">
   <si>
     <t>Name:</t>
   </si>
@@ -1276,54 +1277,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>60:</t>
-  </si>
-  <si>
-    <t>61:</t>
-  </si>
-  <si>
-    <t>62:</t>
-  </si>
-  <si>
-    <t>63:</t>
-  </si>
-  <si>
-    <t>64:</t>
-  </si>
-  <si>
-    <t>65:</t>
-  </si>
-  <si>
-    <t>66:</t>
-  </si>
-  <si>
-    <t>67:</t>
-  </si>
-  <si>
-    <t>68:</t>
-  </si>
-  <si>
-    <t>69:</t>
-  </si>
-  <si>
-    <t>70:</t>
-  </si>
-  <si>
-    <t>71:</t>
-  </si>
-  <si>
-    <t>72:</t>
-  </si>
-  <si>
-    <t>73:</t>
-  </si>
-  <si>
-    <t>74:</t>
-  </si>
-  <si>
-    <t>75:</t>
-  </si>
-  <si>
     <t>76:</t>
   </si>
   <si>
@@ -1895,10 +1848,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>資源事件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>007</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2027,6 +1976,328 @@
   </si>
   <si>
     <t>這個變數用來決定地圖陷阱:1-10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資源事件-石頭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資源事件-木材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MistForestB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>35x40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>森林背景01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>031</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>森林背景02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>039</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖出入口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>039</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0002: TownHallLevel</t>
+  </si>
+  <si>
+    <t>0002: TownHallLevel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖參數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資源事件-石頭</t>
+  </si>
+  <si>
+    <t>001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>資源事件-木材</t>
+  </si>
+  <si>
+    <t>033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>035</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0060:MForestB_EV005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0061:MForestB_EV006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寶箱</t>
+  </si>
+  <si>
+    <t>地圖事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>035</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>035</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://peritune.com/freematerial_list/</t>
+  </si>
+  <si>
+    <t>0062:MForestB_EV007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0063:MForestB_EV008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0064:MForestB_EV009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0065:MForestB_EV010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0066:MForestB_EV011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0067:MForestB_EV012</t>
+  </si>
+  <si>
+    <t>0067:MForestB_EV012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0068:MForestB_EV013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0069:MForestB_EV014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0070:MForestB_EV015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0071:MForestB_EV016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0072:MForestB_EV017</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0073:MForestB_EV018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0074:MForestB_EV019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>035</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>028</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>030</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>019</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>016</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0062:MForestB_EV007</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0063:MForestB_EV008</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0064:MForestB_EV009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0065:MForestB_EV010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傳送-洞口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>傳送-洞口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寶箱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0075:MForestB_EV020</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2076,7 +2347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2116,14 +2387,24 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2857,7 +3138,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2935,7 +3216,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>262</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3284,17 +3565,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="13"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" style="5" customWidth="1"/>
   </cols>
@@ -3304,7 +3585,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3312,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3320,7 +3601,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3351,7 +3632,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>45</v>
@@ -3367,13 +3648,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>463</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>467</v>
+        <v>447</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3381,13 +3662,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>464</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>468</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>469</v>
+        <v>448</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3395,13 +3676,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>465</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>469</v>
+        <v>449</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3409,13 +3690,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>485</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>480</v>
+        <v>469</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3423,16 +3704,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>481</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>482</v>
+        <v>465</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>466</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3440,13 +3721,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>484</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>479</v>
-      </c>
-      <c r="D12" s="13" t="s">
         <v>468</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3454,49 +3735,51 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>486</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>487</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
         <v>287</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>509</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>488</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>488</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="B14" s="16" t="s">
+        <v>492</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>472</v>
+      </c>
+      <c r="E14" s="18"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>288</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>493</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>492</v>
+        <v>475</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="15" t="s">
+        <v>477</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3504,208 +3787,239 @@
         <v>289</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>490</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>510</v>
-      </c>
-      <c r="G16" s="16"/>
+        <v>475</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>474</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="15" t="s">
+        <v>493</v>
+      </c>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>290</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>503</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>511</v>
-      </c>
-      <c r="G17" s="16"/>
+        <v>475</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>486</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="15" t="s">
+        <v>494</v>
+      </c>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>504</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>505</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>512</v>
-      </c>
-      <c r="G18" s="16"/>
+        <v>475</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>487</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>488</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="15" t="s">
+        <v>495</v>
+      </c>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>513</v>
-      </c>
-      <c r="G19" s="16"/>
+        <v>475</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>489</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>490</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="15" t="s">
+        <v>496</v>
+      </c>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>463</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>491</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>508</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>514</v>
-      </c>
-      <c r="G20" s="16"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="15" t="s">
+        <v>497</v>
+      </c>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="D21" s="15" t="s">
+        <v>475</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>480</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>515</v>
-      </c>
-      <c r="G21" s="16"/>
+      <c r="D21" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="E21" s="19"/>
+      <c r="F21" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>502</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="G22" s="16"/>
+        <v>475</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>491</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>495</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>517</v>
-      </c>
-      <c r="G23" s="16"/>
+      <c r="C23" s="21" t="s">
+        <v>479</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>480</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="15" t="s">
+        <v>500</v>
+      </c>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="B24" t="s">
-        <v>497</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>498</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>469</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>518</v>
+        <v>481</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="B25" t="s">
-        <v>497</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>499</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>496</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>519</v>
+        <v>481</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
       <c r="B26" t="s">
-        <v>500</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>520</v>
+        <v>517</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>521</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>508</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>522</v>
+        <v>504</v>
+      </c>
+      <c r="B27" t="s">
+        <v>518</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>526</v>
+      </c>
+      <c r="B28" t="s">
+        <v>527</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -3717,10 +4031,443 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="17.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>524</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>531</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="G8" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>537</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>539</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>542</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>547</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" t="s">
+        <v>548</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" t="s">
+        <v>548</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" t="s">
+        <v>475</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>475</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>454</v>
+      </c>
+      <c r="B18" t="s">
+        <v>475</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>455</v>
+      </c>
+      <c r="B19" t="s">
+        <v>475</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>456</v>
+      </c>
+      <c r="B20" t="s">
+        <v>475</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>457</v>
+      </c>
+      <c r="B21" t="s">
+        <v>475</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>458</v>
+      </c>
+      <c r="B22" t="s">
+        <v>475</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>459</v>
+      </c>
+      <c r="B23" t="s">
+        <v>475</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>460</v>
+      </c>
+      <c r="B24" t="s">
+        <v>475</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>461</v>
+      </c>
+      <c r="B25" t="s">
+        <v>593</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>462</v>
+      </c>
+      <c r="B26" t="s">
+        <v>594</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>504</v>
+      </c>
+      <c r="B27" t="s">
+        <v>597</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3739,34 +4486,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3806,471 +4553,471 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>447</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>449</v>
+        <v>433</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>451</v>
+        <v>435</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>453</v>
+        <v>437</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>327</v>
+        <v>545</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>328</v>
+        <v>546</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>329</v>
+        <v>558</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>330</v>
+        <v>559</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>331</v>
+        <v>560</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>332</v>
+        <v>561</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>333</v>
+        <v>562</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>334</v>
+        <v>564</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>335</v>
+        <v>565</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>336</v>
+        <v>566</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>337</v>
+        <v>567</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>338</v>
+        <v>568</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>339</v>
+        <v>569</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>340</v>
+        <v>570</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>341</v>
+        <v>571</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>342</v>
+        <v>598</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4279,11 +5026,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -4336,10 +5083,10 @@
         <v>206</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4347,10 +5094,10 @@
         <v>207</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4358,10 +5105,10 @@
         <v>208</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4369,10 +5116,10 @@
         <v>209</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4380,10 +5127,10 @@
         <v>210</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4391,10 +5138,10 @@
         <v>211</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -4581,135 +5328,135 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="B42" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="C42" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="B43" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="C43" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B44" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="C44" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -4719,11 +5466,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4733,6 +5482,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>557</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add new tireset to the project -Add MystForestC map -Add events on the MystForestC map -Update Godness bust and show in the conversation window -Update SwitchVariable Excel file
</commit_message>
<xml_diff>
--- a/SwitchVariableConf.xlsx
+++ b/SwitchVariableConf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -23,16 +23,17 @@
     <sheet name="Church_lv2" sheetId="14" r:id="rId14"/>
     <sheet name="MystForestA" sheetId="15" r:id="rId15"/>
     <sheet name="MystForestB" sheetId="19" r:id="rId16"/>
-    <sheet name="Switch" sheetId="12" r:id="rId17"/>
-    <sheet name="Variables" sheetId="17" r:id="rId18"/>
-    <sheet name="resource" sheetId="18" r:id="rId19"/>
+    <sheet name="MystForestC" sheetId="20" r:id="rId17"/>
+    <sheet name="Switch" sheetId="12" r:id="rId18"/>
+    <sheet name="Variables" sheetId="17" r:id="rId19"/>
+    <sheet name="resource" sheetId="18" r:id="rId20"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="698">
   <si>
     <t>Name:</t>
   </si>
@@ -1277,27 +1278,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>76:</t>
-  </si>
-  <si>
-    <t>77:</t>
-  </si>
-  <si>
-    <t>78:</t>
-  </si>
-  <si>
-    <t>79:</t>
-  </si>
-  <si>
-    <t>80:</t>
-  </si>
-  <si>
-    <t>81:</t>
-  </si>
-  <si>
-    <t>82:</t>
-  </si>
-  <si>
     <t>83:</t>
   </si>
   <si>
@@ -2298,6 +2278,386 @@
   </si>
   <si>
     <t>0075:MForestB_EV020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MistForestC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>45x45</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV023</t>
+  </si>
+  <si>
+    <t>EV024</t>
+  </si>
+  <si>
+    <t>EV025</t>
+  </si>
+  <si>
+    <t>EV026</t>
+  </si>
+  <si>
+    <t>EV027</t>
+  </si>
+  <si>
+    <t>EV028</t>
+  </si>
+  <si>
+    <t>EV029</t>
+  </si>
+  <si>
+    <t>EV030</t>
+  </si>
+  <si>
+    <t>阻擋-神殿</t>
+  </si>
+  <si>
+    <t>阻擋-神殿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>025</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0076:RecoverSNStatue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 玩家修復女神像使橋上升通往湖中的島</t>
+  </si>
+  <si>
+    <t>隱藏-橋1</t>
+  </si>
+  <si>
+    <t>隱藏-橋1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隱藏-橋2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>020</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0076:RecoverSNStatue</t>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>009</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV031</t>
+  </si>
+  <si>
+    <t>EV032</t>
+  </si>
+  <si>
+    <t>EV033</t>
+  </si>
+  <si>
+    <t>EV034</t>
+  </si>
+  <si>
+    <t>EV035</t>
+  </si>
+  <si>
+    <t>EV036</t>
+  </si>
+  <si>
+    <t>EV037</t>
+  </si>
+  <si>
+    <t>EV038</t>
+  </si>
+  <si>
+    <t>EV039</t>
+  </si>
+  <si>
+    <t>EV040</t>
+  </si>
+  <si>
+    <t>EV041</t>
+  </si>
+  <si>
+    <t>EV042</t>
+  </si>
+  <si>
+    <t>EV043</t>
+  </si>
+  <si>
+    <t>EV044</t>
+  </si>
+  <si>
+    <t>EV045</t>
+  </si>
+  <si>
+    <t>EV046</t>
+  </si>
+  <si>
+    <t>EV047</t>
+  </si>
+  <si>
+    <t>EV048</t>
+  </si>
+  <si>
+    <t>EV049</t>
+  </si>
+  <si>
+    <t>EV050</t>
+  </si>
+  <si>
+    <t>隱藏-橋3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隱藏-橋4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>034</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>034</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>023</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>033</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>032</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0077:RecoverEWStatue</t>
+  </si>
+  <si>
+    <t>0077:RecoverEWStatue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>031</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隱藏-橋蹾3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隱藏-橋蹾4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>043</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0076:RecoverSNStatue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0077:RecoverEWStatue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0078:MystFCurseSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0079:MystFCurseEW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖參數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0080:MForestC_EV047</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地圖事件</t>
+  </si>
+  <si>
+    <t>006</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0080:MForestC_EV047</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0081:MForestC_EV048</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>014</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0082:MForestC_EV051</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0081:MForestC_EV048</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>005</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0076:RecoverSNStatue, 0078:MystFCurseSN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>021</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EV051</t>
+  </si>
+  <si>
+    <t>EV052</t>
+  </si>
+  <si>
+    <t>EV053</t>
+  </si>
+  <si>
+    <t>EV054</t>
+  </si>
+  <si>
+    <t>EV055</t>
+  </si>
+  <si>
+    <t>EV056</t>
+  </si>
+  <si>
+    <t>EV057</t>
+  </si>
+  <si>
+    <t>EV058</t>
+  </si>
+  <si>
+    <t>EV059</t>
+  </si>
+  <si>
+    <t>EV060</t>
+  </si>
+  <si>
+    <t>女神像1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女神像2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修復女神像開啟橋通往湖中島並停止森林詛咒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>029</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>038</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0083:MForestC_EV052</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3216,7 +3576,7 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -3567,7 +3927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -3585,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3593,7 +3953,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3601,7 +3961,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -3632,7 +3992,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>45</v>
@@ -3648,13 +4008,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -3662,13 +4022,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -3676,13 +4036,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -3690,13 +4050,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -3704,16 +4064,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -3721,13 +4081,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3735,13 +4095,13 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -3749,13 +4109,13 @@
         <v>287</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="17"/>
@@ -3766,20 +4126,20 @@
         <v>288</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="15" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3787,17 +4147,17 @@
         <v>289</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="15" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="G16" s="15"/>
     </row>
@@ -3806,220 +4166,220 @@
         <v>290</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="15" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="E18" s="19"/>
       <c r="F18" s="15" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="E19" s="19"/>
       <c r="F19" s="15" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>456</v>
       </c>
-      <c r="B20" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>463</v>
-      </c>
       <c r="D20" s="21" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="E20" s="19"/>
       <c r="F20" s="15" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>457</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>475</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>480</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>464</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="15" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="15" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="15" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B24" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B25" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B26" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B27" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="B28" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="G28" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -4033,8 +4393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4051,7 +4411,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4059,7 +4419,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4098,13 +4458,13 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -4112,10 +4472,10 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>60</v>
@@ -4126,19 +4486,19 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="G8" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -4146,13 +4506,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4160,16 +4520,16 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4177,16 +4537,16 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -4194,16 +4554,16 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4211,16 +4571,16 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -4228,16 +4588,16 @@
         <v>287</v>
       </c>
       <c r="B14" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4245,16 +4605,16 @@
         <v>288</v>
       </c>
       <c r="B15" t="s">
+        <v>541</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>555</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -4262,16 +4622,16 @@
         <v>289</v>
       </c>
       <c r="B16" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4279,180 +4639,180 @@
         <v>290</v>
       </c>
       <c r="B17" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B18" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B19" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B20" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="B21" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B22" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="B23" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B24" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B25" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B26" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B27" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>591</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>598</v>
       </c>
     </row>
   </sheetData>
@@ -4464,10 +4824,973 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.42578125" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
+    <col min="8" max="8" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>603</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>603</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>603</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>603</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>603</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>603</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>603</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" t="s">
+        <v>603</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B15" t="s">
+        <v>602</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>289</v>
+      </c>
+      <c r="B16" t="s">
+        <v>602</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>290</v>
+      </c>
+      <c r="B17" t="s">
+        <v>602</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>447</v>
+      </c>
+      <c r="B18" t="s">
+        <v>602</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>448</v>
+      </c>
+      <c r="B19" t="s">
+        <v>602</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>449</v>
+      </c>
+      <c r="B20" t="s">
+        <v>602</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" t="s">
+        <v>609</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="F21" t="s">
+        <v>606</v>
+      </c>
+      <c r="H21" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>451</v>
+      </c>
+      <c r="B22" t="s">
+        <v>610</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="F22" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>452</v>
+      </c>
+      <c r="B23" t="s">
+        <v>609</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="F23" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>453</v>
+      </c>
+      <c r="B24" t="s">
+        <v>609</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="F24" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>454</v>
+      </c>
+      <c r="B25" t="s">
+        <v>610</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F25" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>455</v>
+      </c>
+      <c r="B26" t="s">
+        <v>610</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="F26" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>497</v>
+      </c>
+      <c r="B27" t="s">
+        <v>640</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="F27" t="s">
+        <v>652</v>
+      </c>
+      <c r="H27" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>594</v>
+      </c>
+      <c r="B28" t="s">
+        <v>640</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F28" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>595</v>
+      </c>
+      <c r="B29" t="s">
+        <v>640</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F29" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>596</v>
+      </c>
+      <c r="B30" t="s">
+        <v>641</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="F30" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>597</v>
+      </c>
+      <c r="B31" t="s">
+        <v>641</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="F31" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>598</v>
+      </c>
+      <c r="B32" t="s">
+        <v>641</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="F32" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>599</v>
+      </c>
+      <c r="B33" t="s">
+        <v>608</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="F33" t="s">
+        <v>613</v>
+      </c>
+      <c r="H33" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>600</v>
+      </c>
+      <c r="B34" t="s">
+        <v>608</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="F34" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>601</v>
+      </c>
+      <c r="B35" t="s">
+        <v>608</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="F35" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>620</v>
+      </c>
+      <c r="B36" t="s">
+        <v>610</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="F36" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>621</v>
+      </c>
+      <c r="B37" t="s">
+        <v>610</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="F37" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>622</v>
+      </c>
+      <c r="B38" t="s">
+        <v>610</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="F38" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>623</v>
+      </c>
+      <c r="B39" t="s">
+        <v>640</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F39" t="s">
+        <v>651</v>
+      </c>
+      <c r="H39" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>624</v>
+      </c>
+      <c r="B40" t="s">
+        <v>640</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="F40" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>625</v>
+      </c>
+      <c r="B41" t="s">
+        <v>640</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F41" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>626</v>
+      </c>
+      <c r="B42" t="s">
+        <v>641</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="F42" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>627</v>
+      </c>
+      <c r="B43" t="s">
+        <v>641</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="F43" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>628</v>
+      </c>
+      <c r="B44" t="s">
+        <v>641</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="F44" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>629</v>
+      </c>
+      <c r="B45" t="s">
+        <v>656</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="F45" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>630</v>
+      </c>
+      <c r="B46" t="s">
+        <v>657</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="F46" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>631</v>
+      </c>
+      <c r="B47" t="s">
+        <v>657</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="F47" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>632</v>
+      </c>
+      <c r="B48" t="s">
+        <v>656</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="F48" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>633</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="E49" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>634</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="E50" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>635</v>
+      </c>
+      <c r="B51" t="s">
+        <v>666</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>636</v>
+      </c>
+      <c r="B52" t="s">
+        <v>669</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="F52" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>637</v>
+      </c>
+      <c r="B53" t="s">
+        <v>669</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="F53" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>638</v>
+      </c>
+      <c r="B54" t="s">
+        <v>692</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="F54" t="s">
+        <v>679</v>
+      </c>
+      <c r="H54" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>639</v>
+      </c>
+      <c r="B55" t="s">
+        <v>693</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F55" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>682</v>
+      </c>
+      <c r="B56" t="s">
+        <v>669</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F56" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>683</v>
+      </c>
+      <c r="B57" t="s">
+        <v>669</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F57" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>691</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4486,34 +5809,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4553,471 +5876,471 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>327</v>
+        <v>662</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>328</v>
+        <v>663</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>329</v>
+        <v>664</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>330</v>
+        <v>665</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>331</v>
+        <v>668</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>332</v>
+        <v>673</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>333</v>
+        <v>675</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -5026,11 +6349,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -5083,10 +6406,10 @@
         <v>206</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5094,10 +6417,10 @@
         <v>207</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5105,10 +6428,10 @@
         <v>208</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5116,10 +6439,10 @@
         <v>209</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5127,10 +6450,10 @@
         <v>210</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5138,10 +6461,10 @@
         <v>211</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -5328,170 +6651,141 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B42" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C42" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B43" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C43" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B44" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C44" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5625,6 +6919,35 @@
       </c>
       <c r="E9" s="2" t="s">
         <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>550</v>
       </c>
     </row>
   </sheetData>

</xml_diff>